<commit_message>
adding in updated gamma cross sections
</commit_message>
<xml_diff>
--- a/gamma_cross_sections/io/inputs/gammaEnergies.xlsx
+++ b/gamma_cross_sections/io/inputs/gammaEnergies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/perrindavidson/Desktop/uchicago/academics/phys_21101/labs/phys21101/gamma_cross_sections/io/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910BCB40-BC0E-2C47-86E0-061C7157C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85396E9-D4A2-EE42-8892-34DC1B6A7041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1440" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{82F59CDD-3AD1-ED41-9A89-569E6757C999}"/>
   </bookViews>
@@ -9067,8 +9067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCF6C97-C150-5640-9F1D-E7D62749746C}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>